<commit_message>
third day and data manipulation is finished, raw components to show data created
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD11DC7-CAA5-4057-BF65-E2A4FC3C63FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAF48C6-268B-4BDA-BE43-A1D9B470F9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>päivä</t>
   </si>
   <si>
-    <t>aika</t>
-  </si>
-  <si>
     <t>mitä tein</t>
   </si>
   <si>
@@ -106,6 +103,36 @@
   </si>
   <si>
     <t>datan muokkausta ja kokeilua API:lta ladatulta esimerkki-response:lla</t>
+  </si>
+  <si>
+    <t>päivämäärä-listan tarkistus ja korjaus, 00:00 muuttui automaattisesti muotoon 23:00</t>
+  </si>
+  <si>
+    <t>ensimmäinen datan muokkausfunktio tehty, yksi datapiste per päivä, lähin keskiyöltä, getOneDataPointPerDate</t>
+  </si>
+  <si>
+    <t>toinen datan muokkausfuntio tehty, pisin 'bearish trend' haetualla aikavälillä, getLongestBearishTrend</t>
+  </si>
+  <si>
+    <t>kolmas muokkausfuntio tehty, suurin volyymi päivä, funktioiden pientä refaktotorointia, forEach ==&gt; map, tarkemmat nimet</t>
+  </si>
+  <si>
+    <t>aika(h)</t>
+  </si>
+  <si>
+    <t>neljäs muokkausfuntio tehty, paras päivä ostaa ja myydä, eli suurin profit</t>
+  </si>
+  <si>
+    <t>edellisen funktion korjausta testausta eri sarjoilla</t>
+  </si>
+  <si>
+    <t>same date error lisätty, perus data näkyy bearish trend, highest trading volume, best buy/sell</t>
+  </si>
+  <si>
+    <t>Dataview sisällön perustan luonti, hardcoded data testaukseen</t>
+  </si>
+  <si>
+    <t>refaktorointia uusien komponenttien kanssa, funktioiden testausta, kommentoinnin korjausta ja lisäystä</t>
   </si>
 </sst>
 </file>
@@ -472,17 +499,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="107.85546875" customWidth="1"/>
+    <col min="3" max="3" width="115.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -490,10 +517,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -520,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,7 +563,7 @@
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +595,7 @@
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -584,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -611,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,21 +686,91 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>44532</v>
       </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="B30" s="1">
-        <f>SUM(B2:B21)</f>
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <f>SUM(B2:B30)</f>
+        <v>33.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fourth day behind, css basic styling, final testing for input to dataview, cleaning code todo
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAF48C6-268B-4BDA-BE43-A1D9B470F9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A864891-8CA6-4716-838D-6F1EBF073B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="3345" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>päivä</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t>refaktorointia uusien komponenttien kanssa, funktioiden testausta, kommentoinnin korjausta ja lisäystä</t>
+  </si>
+  <si>
+    <t>3.21.2021</t>
+  </si>
+  <si>
+    <t>refaktorointia, error viestien resetointi Reset napilla, nimien lyhentämistä, DataView komponenttien useEffect</t>
+  </si>
+  <si>
+    <t>DataView css ja näkymän parantelua</t>
+  </si>
+  <si>
+    <t>datan parserit jotta luvut ja päivät näkyy halutulla/siistimmällä tavalla</t>
+  </si>
+  <si>
+    <t>parserit yhteiseen käyttöön utils/functions.js, css väritystä</t>
+  </si>
+  <si>
+    <t>kaikki perustoiminnot saatu toimimaan, date input, fetch, datan manipulointi, datan esittely, perus css</t>
+  </si>
+  <si>
+    <t>ajax funktio luotu, axios implementation myöhemmin</t>
   </si>
 </sst>
 </file>
@@ -499,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,11 +787,62 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="1">
-        <f>SUM(B2:B30)</f>
-        <v>33.5</v>
+      <c r="B37" s="1">
+        <f>SUM(B2:B36)</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validation korjausta, Docker kuva ja kontin testaus, kontti Herokuun testi, workflowt push to main tapahtumalle
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A864891-8CA6-4716-838D-6F1EBF073B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBFF0E0-F803-442E-99C5-37AE14DA8DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>päivä</t>
   </si>
@@ -150,10 +150,25 @@
     <t>parserit yhteiseen käyttöön utils/functions.js, css väritystä</t>
   </si>
   <si>
-    <t>kaikki perustoiminnot saatu toimimaan, date input, fetch, datan manipulointi, datan esittely, perus css</t>
-  </si>
-  <si>
     <t>ajax funktio luotu, axios implementation myöhemmin</t>
+  </si>
+  <si>
+    <t>perustoimintojen alustava viimeistely, date input=&gt; fetch=&gt; datan manipulointi=&gt; datan esittely=&gt; perus css</t>
+  </si>
+  <si>
+    <t>pientä css tuunausta ja testifunktioiden siivousta</t>
+  </si>
+  <si>
+    <t>rakenteen refaktorin, Loading komponentti ja turhat statet pois, 'ylimääräiset' useEffect hookit pois</t>
+  </si>
+  <si>
+    <t>Docker image(production testi) ja testiajoa kontissa</t>
+  </si>
+  <si>
+    <t>CI/CD push to github main =&gt; uusi kuva dockerhubiin</t>
+  </si>
+  <si>
+    <t>Heroku app, workflow push github main =&gt; uusi appi Herokuun</t>
   </si>
 </sst>
 </file>
@@ -520,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,16 +848,62 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="5">
+        <v>44534</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>44535</v>
+      </c>
+      <c r="B38" s="1">
         <v>2</v>
       </c>
-      <c r="B37" s="1">
-        <f>SUM(B2:B36)</f>
-        <v>40</v>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1">
+        <f>SUM(B2:B41)</f>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created placeholders for next features, login and navbar, basic css and components added
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E463022-D962-473C-BA75-979E2400973C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9542BC-A385-4398-B0B4-387A17E799F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>päivä</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>reserve proxy + backend + front herokuun -asetukset  ja ohjeistus käyty läpi</t>
+  </si>
+  <si>
+    <t>ilmettä uusittu, login ja navbar placeholderit lisätty ja komponentit luotu</t>
+  </si>
+  <si>
+    <t>css refaktorin, css tiedosto refaktorin todo huomenna</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
@@ -919,13 +925,32 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>44536</v>
+      </c>
+      <c r="B44" s="1">
         <v>2</v>
       </c>
-      <c r="B44" s="1">
-        <f>SUM(B2:B43)</f>
-        <v>48.5</v>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="1">
+        <f>SUM(B2:B45)</f>
+        <v>51.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small tweaks, mainly tuntikirjanpito
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4328D7F5-7588-4F4D-8B33-BB97EA960A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1919A8-C5CB-44B1-856E-40247625D51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="4380" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>päivä</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>eslint ja asetukset, lintattu frontti ja koodin bugien korjausta</t>
+  </si>
+  <si>
+    <t>backend perus error handling, logging tehty</t>
+  </si>
+  <si>
+    <t>backend pari scheemaa, perusasetuksia, user ja favoriteDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usersRouter, error handling </t>
+  </si>
+  <si>
+    <t>asynchandler, usersRouter testausta ja errorien läpikäyntiä</t>
+  </si>
+  <si>
+    <t>dev ympäristön alustaminen, docker =&gt; konttiin backend + mongodb</t>
+  </si>
+  <si>
+    <t>dev ympäristön luotu loppuun, muutokset päivittyy suoraan konttiin, mongodb pyörii kontissa ongelmitta</t>
   </si>
 </sst>
 </file>
@@ -559,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,16 +1128,86 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>44537</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
         <v>2</v>
       </c>
-      <c r="B50" s="1">
-        <f>SUM(B2:B47)</f>
-        <v>55.5</v>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="1">
+        <f>SUM(B2:B53)</f>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code refactoring and first redux implementation steps
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B992D-48A2-4737-B458-CAE82C009A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C728A1-8C61-4B56-B122-2ADDD58EE967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30555" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t>päivä</t>
   </si>
@@ -226,6 +226,24 @@
   </si>
   <si>
     <t>mongoose custom validator dokumentoinnin lukemista ja harjoittelua</t>
+  </si>
+  <si>
+    <t>login form luotu, router lisätty jotta navigointia voidaan käyttää, analyzer container datan hakuun luotu</t>
+  </si>
+  <si>
+    <t>redux perusasetukset tehty, ekan analyzerReducer rakentamista</t>
+  </si>
+  <si>
+    <t>error reducer tehty ja koodin refaktorointia ja testausta</t>
+  </si>
+  <si>
+    <t>login form css ja statet muokattu</t>
+  </si>
+  <si>
+    <t>oma uudelleenkäytettävä komponentti formien submit/cancel napeille, css luokkien uudelleen nimeämistä</t>
+  </si>
+  <si>
+    <t>loginservice luotu, ei testattu, userReducer ja lisäys storeen</t>
   </si>
 </sst>
 </file>
@@ -592,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,13 +1291,85 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>2</v>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>44565</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>44567</v>
       </c>
       <c r="B60" s="1">
-        <f>SUM(B2:B58)</f>
-        <v>71</v>
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="1">
+        <f>SUM(B2:B64)</f>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first phase of login done, clientside form and service, apiside cookie forming and authentication refactoring
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C728A1-8C61-4B56-B122-2ADDD58EE967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE7DC6A-2E3F-4F84-853C-C0ED6EC41C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>päivä</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>loginservice luotu, ei testattu, userReducer ja lisäys storeen</t>
+  </si>
+  <si>
+    <t>route tokenin tarkistukseen</t>
+  </si>
+  <si>
+    <t>opeteltuauth  cookien lähettäminen suoraan serveriltä, testattu ja apin:n koodi refaktoroitu</t>
   </si>
 </sst>
 </file>
@@ -612,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,13 +1369,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>44571</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>44572</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B64)</f>
-        <v>78</v>
+        <f>SUM(B2:B66)</f>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2nd phase of login settings with minor additions to signup and logout
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE7DC6A-2E3F-4F84-853C-C0ED6EC41C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3427029B-881E-4544-8200-DAFA9B90067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
   <si>
     <t>päivä</t>
   </si>
@@ -249,7 +249,10 @@
     <t>route tokenin tarkistukseen</t>
   </si>
   <si>
-    <t>opeteltuauth  cookien lähettäminen suoraan serveriltä, testattu ja apin:n koodi refaktoroitu</t>
+    <t>opeteltu auth  cookien lähettäminen suoraan serveriltä, testattu ja apin:n koodi refaktoroitu</t>
+  </si>
+  <si>
+    <t>api herokuun, github action automaattiseen liven päivittämiseen, production versiossa oma mongodb url(ei omaa konttia)</t>
   </si>
 </sst>
 </file>
@@ -618,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,13 +1400,24 @@
         <v>51</v>
       </c>
     </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B66)</f>
-        <v>81</v>
+        <f>SUM(B2:B67)</f>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
live versions for client and api are somewhat working, not great not terrible
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3427029B-881E-4544-8200-DAFA9B90067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758196F4-A60D-4C53-99D3-838797B1E869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="885" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
   <si>
     <t>päivä</t>
   </si>
@@ -253,6 +253,15 @@
   </si>
   <si>
     <t>api herokuun, github action automaattiseen liven päivittämiseen, production versiossa oma mongodb url(ei omaa konttia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client login, logout ja signup pohja, cookie pohjainen permanent login lisätty </t>
+  </si>
+  <si>
+    <t>api/client</t>
+  </si>
+  <si>
+    <t>heroku live testausta, client ja api livenä ja toimii jotenkin(login hidas), not great, not terrible</t>
   </si>
 </sst>
 </file>
@@ -621,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,13 +1420,35 @@
         <v>51</v>
       </c>
     </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>73</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>75</v>
+      </c>
+      <c r="D69" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B67)</f>
-        <v>84</v>
+        <f>SUM(B2:B69)</f>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
signup half working, errors and auto login missing, refactored new TextInput component
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758196F4-A60D-4C53-99D3-838797B1E869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8850C2D-8BF5-40DF-8BE1-EE8025A4E9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
   <si>
     <t>päivä</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>heroku live testausta, client ja api livenä ja toimii jotenkin(login hidas), not great, not terrible</t>
+  </si>
+  <si>
+    <t>login ja signup for refaktoroitu, uusi TextInput komponentti, signup formista puuttuu vielä errorit, signup service</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,13 +1445,24 @@
         <v>74</v>
       </c>
     </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B69)</f>
-        <v>87</v>
+        <f>SUM(B2:B70)</f>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
login last phase done, cookie check from api, signup clean and working now
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8850C2D-8BF5-40DF-8BE1-EE8025A4E9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D471888-3DA3-43DE-B6CC-67F0F198B69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
   <si>
     <t>päivä</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>login ja signup for refaktoroitu, uusi TextInput komponentti, signup formista puuttuu vielä errorit, signup service</t>
+  </si>
+  <si>
+    <t>signup form refaktorointia, lisätty kenttä 'retype password', otsikko, auto-login, validointi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otsikot lisätty kaikkiin formeihin, signup testattu ja toimii, login kolmas ja viimeinen vaihe implementoitu, token cookie tarkistus </t>
   </si>
 </sst>
 </file>
@@ -634,7 +640,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,13 +1462,38 @@
         <v>51</v>
       </c>
     </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>44573</v>
+      </c>
+      <c r="B71" s="1">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>77</v>
+      </c>
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>78</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B70)</f>
-        <v>89</v>
+        <f>SUM(B2:B72)</f>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comments added and refactored to keep things more clean, /home started
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D471888-3DA3-43DE-B6CC-67F0F198B69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085449BB-ED2C-4992-B4B7-CE503E614CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
   <si>
     <t>päivä</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t xml:space="preserve">otsikot lisätty kaikkiin formeihin, signup testattu ja toimii, login kolmas ja viimeinen vaihe implementoitu, token cookie tarkistus </t>
+  </si>
+  <si>
+    <t>kommenttien lisäystä melkein kaikkiin komponentteihin, myös vääriä kommentteja korjattu, pientä refaktorointia</t>
+  </si>
+  <si>
+    <t>/home pohja, Info ja TopCoins aloitettu</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,13 +1493,38 @@
         <v>49</v>
       </c>
     </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>44574</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B72)</f>
-        <v>93</v>
+        <f>SUM(B2:B74)</f>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
css fixes and componentWillUnmount to Dataview component for data reset to redux store
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085449BB-ED2C-4992-B4B7-CE503E614CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E3CA6-76C2-4511-B997-F827E0E84870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="29685" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
   <si>
     <t>päivä</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>/home pohja, Info ja TopCoins aloitettu</t>
+  </si>
+  <si>
+    <t>pientä css tuunausta, suuremmat fontit jne, Dataview komponenttiin redux storen resetointi componentWillUnmount avulla</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,13 +1521,27 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>2</v>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>44575</v>
       </c>
       <c r="B75" s="1">
-        <f>SUM(B2:B74)</f>
-        <v>95</v>
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="1">
+        <f>SUM(B2:B75)</f>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
market page created and Top Coins moved, small changes to login and navbar visibility
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E3CA6-76C2-4511-B997-F827E0E84870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98943FD-2890-41DD-BACF-B73A92D5601E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29685" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="3855" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
   <si>
     <t>päivä</t>
   </si>
@@ -280,6 +280,18 @@
   </si>
   <si>
     <t>pientä css tuunausta, suuremmat fontit jne, Dataview komponenttiin redux storen resetointi componentWillUnmount avulla</t>
+  </si>
+  <si>
+    <t>NavBar profile näkyy vain kun käyttäjä kirjautuneena, TopCoins siirretty ja uudelleennimetty Market sivulle</t>
+  </si>
+  <si>
+    <t>uusi Gecko API linkki haettu ja testattu, top 5 kolikot market cap, hinta per coin, volume</t>
+  </si>
+  <si>
+    <t>Market sivun komponettien pohjien rakentelua, CoinCard, CoinCardList, NoData, MarketContainer</t>
+  </si>
+  <si>
+    <t>CoinCard tuunausta, Font Awsome -kirjaston lisäys</t>
   </si>
 </sst>
 </file>
@@ -649,7 +661,7 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,13 +1547,60 @@
         <v>49</v>
       </c>
     </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>44578</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>85</v>
+      </c>
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B86" s="1">
-        <f>SUM(B2:B75)</f>
-        <v>96</v>
+        <f>SUM(B2:B79)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error message refactored to notification and new features added to login and sign up
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98943FD-2890-41DD-BACF-B73A92D5601E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0BA2FF-6F03-4082-8D2C-2A491479D5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
   <si>
     <t>päivä</t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>CoinCard tuunausta, Font Awsome -kirjaston lisäys</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>suoritettu(%)</t>
+  </si>
+  <si>
+    <t>errorMessage komponentti muutettu Notification yleiskomponentiksi  (error, success, action jaot), reducer muokattu</t>
+  </si>
+  <si>
+    <t>Notification otettu käyttöön Login ja Sign Up komponenteissa laajemmin, muissa error osio käytössä normaalisti</t>
   </si>
 </sst>
 </file>
@@ -658,15 +670,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="115.140625" customWidth="1"/>
   </cols>
@@ -1594,13 +1606,52 @@
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B86" s="1">
-        <f>SUM(B2:B79)</f>
-        <v>100</v>
+        <f>SUM(B2:B81)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1">
+        <f>B86/B87*100</f>
+        <v>58.285714285714285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
currency and coin options for analyzer, new options included in DataView also
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0BA2FF-6F03-4082-8D2C-2A491479D5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0071D085-BBC3-4FF7-AA92-31D60FB2A44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="92">
   <si>
     <t>päivä</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Notification otettu käyttöön Login ja Sign Up komponenteissa laajemmin, muissa error osio käytössä normaalisti</t>
+  </si>
+  <si>
+    <t>Kaksi uutta hakukenttää Analyzer työkaluun, parametrien selvittelyä ja yhteisen komponentin DropDownMenu luonti</t>
+  </si>
+  <si>
+    <t>uusien hakukenttien käyttöönotto haussa, datan näyttäminen uusien arvojen avulla, DataView komponentit</t>
   </si>
 </sst>
 </file>
@@ -673,7 +679,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,13 +1634,35 @@
         <v>49</v>
       </c>
     </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="1">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>91</v>
+      </c>
+      <c r="D83" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B86" s="1">
-        <f>SUM(B2:B81)</f>
-        <v>102</v>
+        <f>SUM(B2:B83)</f>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,7 +1679,7 @@
       </c>
       <c r="B88" s="1">
         <f>B86/B87*100</f>
-        <v>58.285714285714285</v>
+        <v>60.571428571428577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small visual tuning for analyzer form, logos for coins, small code refactoring
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0071D085-BBC3-4FF7-AA92-31D60FB2A44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E1356-75FD-4409-AFE3-3FC8E9C12F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="93">
   <si>
     <t>päivä</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>uusien hakukenttien käyttöönotto haussa, datan näyttäminen uusien arvojen avulla, DataView komponentit</t>
+  </si>
+  <si>
+    <t>punta lisätty valuuttoihin, uusien komponenttien siistimistä, analyzer työkalun css yhdenmukaiseksi, coin logot</t>
   </si>
 </sst>
 </file>
@@ -676,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,30 +1659,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="1">
-        <f>SUM(B2:B83)</f>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>44579</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="1">
+        <f>SUM(B2:B84)</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B97" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="1">
-        <f>B86/B87*100</f>
-        <v>60.571428571428577</v>
+      <c r="B98" s="1">
+        <f>B96/B97*100</f>
+        <v>61.142857142857146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataview refactored to make it more clean
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A54183-49A9-4AEA-B0D8-A48F3EC29A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3BB1D7-423A-4F7D-AA44-1A9F9D95C211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
   <si>
     <t>päivä</t>
   </si>
@@ -322,6 +322,15 @@
   </si>
   <si>
     <t>routes api/favorites post ja get all testattu, suosikit tallentuu myös käyttäjän 'favorites' listaan</t>
+  </si>
+  <si>
+    <t>analyzer form info, home info kirjoitusta</t>
+  </si>
+  <si>
+    <t>DataView Refaktorointi, 3 uutta reduceria, componentteja siistitty niin että logiikkaa siirretty pois komponentista</t>
+  </si>
+  <si>
+    <t>Market css refaktorointia, toimintojen testausta, kaikki toimii muutosten jälkeen</t>
   </si>
 </sst>
 </file>
@@ -691,7 +700,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,13 +1713,49 @@
         <v>51</v>
       </c>
     </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>44585</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D87" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="1">
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
+        <v>97</v>
+      </c>
+      <c r="D88" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="1">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>98</v>
+      </c>
+      <c r="D89" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B96" s="1">
-        <f>SUM(B2:B86)</f>
-        <v>109</v>
+        <f>SUM(B2:B89)</f>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1727,7 +1772,7 @@
       </c>
       <c r="B98" s="1">
         <f>B96/B97*100</f>
-        <v>62.285714285714292</v>
+        <v>65.142857142857153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
favorite add button added to analyzer form, profile page building started, service created and tested for profile
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3BB1D7-423A-4F7D-AA44-1A9F9D95C211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6856E4E0-79BE-444B-888A-3A8AFD722803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="1875" yWindow="2235" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
   <si>
     <t>päivä</t>
   </si>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>Market css refaktorointia, toimintojen testausta, kaikki toimii muutosten jälkeen</t>
+  </si>
+  <si>
+    <t>client/api</t>
+  </si>
+  <si>
+    <t>/api/users/:id route tehty ja testattu</t>
+  </si>
+  <si>
+    <t>Analyzer save nappi ja profiilin pohjan rakenne, backend korjaus ('validoi' vahingossa käyttäjän)</t>
+  </si>
+  <si>
+    <t>favoriteService, ongelmat 'populate' kohdassa API:n kanssa korjattu, tuo oikean datan, testattu</t>
   </si>
 </sst>
 </file>
@@ -699,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,13 +1761,46 @@
         <v>49</v>
       </c>
     </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="1">
+        <v>3</v>
+      </c>
+      <c r="C90" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="1">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>100</v>
+      </c>
+      <c r="D91" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="1">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B96" s="1">
-        <f>SUM(B2:B89)</f>
-        <v>114</v>
+        <f>SUM(B2:B92)</f>
+        <v>119</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1772,7 +1817,7 @@
       </c>
       <c r="B98" s="1">
         <f>B96/B97*100</f>
-        <v>65.142857142857153</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PrivateRoute, Authenticate components working, refresh fixed, should redirect to correct page
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6856E4E0-79BE-444B-888A-3A8AFD722803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE89303-E3AA-4308-96E1-6860B9596DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="2235" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="31740" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="107">
   <si>
     <t>päivä</t>
   </si>
@@ -343,6 +343,18 @@
   </si>
   <si>
     <t>favoriteService, ongelmat 'populate' kohdassa API:n kanssa korjattu, tuo oikean datan, testattu</t>
+  </si>
+  <si>
+    <t>väärä käyttäjä/omistaja error lisätty /api/users/:id, /profile sivun 'refresh' korjattu</t>
+  </si>
+  <si>
+    <t>Authenticate, Forbidden komponentit tehty, App siivottu, automaattisesti takaisin aikaisemmalle sivulle login jälkeen</t>
+  </si>
+  <si>
+    <t>PrivateRoute testausta, vanha tapa ei toimi react-router v6:ssa</t>
+  </si>
+  <si>
+    <t>uusi tapa, wrapper toiminnassa,  refresh saatu taas toimimaan private routen kanssa</t>
   </si>
 </sst>
 </file>
@@ -709,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,30 +1806,77 @@
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>2</v>
-      </c>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>44586</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>103</v>
+      </c>
+      <c r="D93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="1">
+        <v>3</v>
+      </c>
+      <c r="C94" t="s">
+        <v>104</v>
+      </c>
+      <c r="D94" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="1">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>105</v>
+      </c>
+      <c r="D95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="1">
-        <f>SUM(B2:B92)</f>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>106</v>
+      </c>
+      <c r="D96" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="1">
+        <f>SUM(B2:B96)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B102" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B98" s="1">
-        <f>B96/B97*100</f>
-        <v>68</v>
+      <c r="B103" s="1">
+        <f>B101/B102*100</f>
+        <v>72.571428571428569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BEM and Sass conversion started, half done
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECCDB9E-B216-4CB3-A58C-E3A09137B6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF10DBFD-C58B-4EC8-A7F0-E187A5D95211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="3720" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="120">
   <si>
     <t>päivä</t>
   </si>
@@ -376,6 +376,24 @@
   </si>
   <si>
     <t>/profile täytetty loppuun, data päivittyy oikein/heti näkyville ilman että sivu pitää ladata</t>
+  </si>
+  <si>
+    <t>tustustuminen sass react dokumentointiin</t>
+  </si>
+  <si>
+    <t>form submit ja reset komponettien erottelu ja scss, SignUpFormCntr jotta keskustelu backending kanssa erillään, extractErrorMsg</t>
+  </si>
+  <si>
+    <t>.scss testaus, import, extend jne, Constants.scss aloitettu</t>
+  </si>
+  <si>
+    <t>loginForm refaktoroitu, scss ja LoginFormCntr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analyzerForm, refaktorointia ja scss, visuaalista tuunausta, </t>
+  </si>
+  <si>
+    <t>analyzerInfo scss ja pientä tuunausta</t>
   </si>
 </sst>
 </file>
@@ -742,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,30 +1972,102 @@
         <v>49</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>2</v>
-      </c>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
+        <v>44588</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="1">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>116</v>
+      </c>
+      <c r="D105" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>44589</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>115</v>
+      </c>
+      <c r="D106" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="1">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>117</v>
+      </c>
+      <c r="D107" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="1">
-        <f>SUM(B2:B103)</f>
-        <v>135</v>
+        <v>3</v>
+      </c>
+      <c r="C108" t="s">
+        <v>118</v>
+      </c>
+      <c r="D108" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+      <c r="B109" s="1">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="1">
+        <f>SUM(B2:B109)</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B113" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B110" s="1">
-        <f>B108/B109*100</f>
-        <v>77.142857142857153</v>
+      <c r="B114" s="1">
+        <f>B112/B113*100</f>
+        <v>82.857142857142861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost finished BEM + Sass transition
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF10DBFD-C58B-4EC8-A7F0-E187A5D95211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDD89F8-4F5F-4B8E-BD0D-A145A8603AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="30975" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="122">
   <si>
     <t>päivä</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>analyzerInfo scss ja pientä tuunausta</t>
+  </si>
+  <si>
+    <t>Notification scss, pieniä muutoksia, LoginBar scss</t>
+  </si>
+  <si>
+    <t>Reset, Base, Header, LoginBar loppuun, Nav, Footer, Loading, Authenticate   scss, mixinien luontia ja kokeilua</t>
   </si>
 </sst>
 </file>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,30 +2050,55 @@
         <v>49</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="1">
-        <f>SUM(B2:B109)</f>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="5">
+        <v>44590</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>120</v>
+      </c>
+      <c r="D110" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="1">
+        <v>3</v>
+      </c>
+      <c r="C111" t="s">
+        <v>121</v>
+      </c>
+      <c r="D111" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="1">
+        <f>SUM(B2:B111)</f>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B116" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B114" s="1">
-        <f>B112/B113*100</f>
-        <v>82.857142857142861</v>
+      <c r="B117" s="1">
+        <f>B115/B116*100</f>
+        <v>85.142857142857139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sass + BEM transition done for everything except Profile, NavBar follows active site now
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDD89F8-4F5F-4B8E-BD0D-A145A8603AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4234FCD-39FF-445D-981D-53336766D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30975" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="3030" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="123">
   <si>
     <t>päivä</t>
   </si>
@@ -399,7 +399,10 @@
     <t>Notification scss, pieniä muutoksia, LoginBar scss</t>
   </si>
   <si>
-    <t>Reset, Base, Header, LoginBar loppuun, Nav, Footer, Loading, Authenticate   scss, mixinien luontia ja kokeilua</t>
+    <t>Reset, Base, Header, LoginBar loppuun, Footer, Loading, Authenticate  scss, mixinien luontia ja kokeilua</t>
+  </si>
+  <si>
+    <t>Buttons, DataView, Home, Inputs, Market, NavBar scss transitio ja muokkaus, NavBar refaktor, seuraa aktiivista sivua</t>
   </si>
 </sst>
 </file>
@@ -769,7 +772,7 @@
   <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,13 +2078,27 @@
         <v>49</v>
       </c>
     </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="5">
+        <v>44591</v>
+      </c>
+      <c r="B112" s="1">
+        <v>6</v>
+      </c>
+      <c r="C112" t="s">
+        <v>122</v>
+      </c>
+      <c r="D112" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="115" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B115" s="1">
-        <f>SUM(B2:B111)</f>
-        <v>149</v>
+        <f>SUM(B2:B112)</f>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2098,7 +2115,7 @@
       </c>
       <c r="B117" s="1">
         <f>B115/B116*100</f>
-        <v>85.142857142857139</v>
+        <v>88.571428571428569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BEM + Sass transition done, small refactoring in style, css removed
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4234FCD-39FF-445D-981D-53336766D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200306E0-D5FA-4E38-ADEC-33F6404BDCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="30585" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="124">
   <si>
     <t>päivä</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Buttons, DataView, Home, Inputs, Market, NavBar scss transitio ja muokkaus, NavBar refaktor, seuraa aktiivista sivua</t>
+  </si>
+  <si>
+    <t>Profile sivun komponentit muutettu käyttämään Sass:ia ja muokattu vähän ilmettä ja koodia</t>
   </si>
 </sst>
 </file>
@@ -772,7 +775,7 @@
   <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,16 +2095,30 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="5">
+        <v>44592</v>
+      </c>
+      <c r="B113" s="1">
+        <v>3</v>
+      </c>
+      <c r="C113" t="s">
+        <v>123</v>
+      </c>
+      <c r="D113" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B115" s="1">
-        <f>SUM(B2:B112)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUM(B2:B113)</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>86</v>
       </c>
@@ -2109,13 +2126,13 @@
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B117" s="1">
         <f>B115/B116*100</f>
-        <v>88.571428571428569</v>
+        <v>90.285714285714278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing setup done, PrivateRoute tests done
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200306E0-D5FA-4E38-ADEC-33F6404BDCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC268CA6-46B9-4B51-A162-42066C959E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30585" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="127">
   <si>
     <t>päivä</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>Profile sivun komponentit muutettu käyttämään Sass:ia ja muokattu vähän ilmettä ja koodia</t>
+  </si>
+  <si>
+    <t>Hook (useSelector, useDispatch) testien selvittelyä ja opiskelua</t>
+  </si>
+  <si>
+    <t>Perusasetusten teko ja jest kirjastojen asennus, ekan testin rakentamista ja errorien korjausta</t>
+  </si>
+  <si>
+    <t>PrivateRoute testit</t>
   </si>
 </sst>
 </file>
@@ -772,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,30 +2118,69 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>2</v>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>124</v>
+      </c>
+      <c r="D114" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="5">
+        <v>44593</v>
       </c>
       <c r="B115" s="1">
-        <f>SUM(B2:B113)</f>
-        <v>158</v>
+        <v>1.5</v>
+      </c>
+      <c r="C115" t="s">
+        <v>125</v>
+      </c>
+      <c r="D115" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="5">
+        <v>44594</v>
+      </c>
+      <c r="B116" s="1">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>126</v>
+      </c>
+      <c r="D116" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="1">
+        <f>SUM(B2:B116)</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B120" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B117" s="1">
-        <f>B115/B116*100</f>
-        <v>90.285714285714278</v>
+      <c r="B121" s="1">
+        <f>B119/B120*100</f>
+        <v>92.571428571428569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notification and LoginBar tests built and testing redux store made to help testing
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC268CA6-46B9-4B51-A162-42066C959E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F796C857-3C9C-4E1B-9FA7-C54BD47A38DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30585" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
   <si>
     <t>päivä</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>PrivateRoute testit</t>
+  </si>
+  <si>
+    <t>Notification tests, redux fake store, store Provider wrapper</t>
+  </si>
+  <si>
+    <t>Loginbar tests</t>
   </si>
 </sst>
 </file>
@@ -781,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2154,7 @@
         <v>44594</v>
       </c>
       <c r="B116" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C116" t="s">
         <v>126</v>
@@ -2157,30 +2163,55 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B119" s="1">
-        <f>SUM(B2:B116)</f>
-        <v>162</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>44595</v>
+      </c>
+      <c r="B117" s="1">
+        <v>3</v>
+      </c>
+      <c r="C117" t="s">
+        <v>127</v>
+      </c>
+      <c r="D117" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="1">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>128</v>
+      </c>
+      <c r="D118" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="1">
+        <f>SUM(B2:B118)</f>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B124" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B121" s="1">
-        <f>B119/B120*100</f>
-        <v>92.571428571428569</v>
+      <c r="B125" s="1">
+        <f>B123/B124*100</f>
+        <v>95.428571428571431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SignUpForm tests done, useDispatch mock working now
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F796C857-3C9C-4E1B-9FA7-C54BD47A38DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4A0C22-1B68-4125-8FEF-5D9EE3F26AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30585" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="130">
   <si>
     <t>päivä</t>
   </si>
@@ -417,10 +417,13 @@
     <t>PrivateRoute testit</t>
   </si>
   <si>
-    <t>Notification tests, redux fake store, store Provider wrapper</t>
-  </si>
-  <si>
-    <t>Loginbar tests</t>
+    <t>SignUpForm testit</t>
+  </si>
+  <si>
+    <t>Loginbar testit</t>
+  </si>
+  <si>
+    <t>Notification testit, redux fake store, store Provider wrapper</t>
   </si>
 </sst>
 </file>
@@ -789,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D117" t="s">
         <v>49</v>
@@ -2188,13 +2191,29 @@
         <v>49</v>
       </c>
     </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="1">
+        <v>4</v>
+      </c>
+      <c r="C119" t="s">
+        <v>127</v>
+      </c>
+      <c r="D119" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="123" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B123" s="1">
-        <f>SUM(B2:B118)</f>
-        <v>167</v>
+        <f>SUM(B2:B119)</f>
+        <v>171</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2211,7 +2230,7 @@
       </c>
       <c r="B125" s="1">
         <f>B123/B124*100</f>
-        <v>95.428571428571431</v>
+        <v>97.714285714285708</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Profile page components testing almost finished, readme and info edited for project submit
</commit_message>
<xml_diff>
--- a/Tuntikirjanpito.xlsx
+++ b/Tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac_na\Documents\GitHub\Vincit-Rising-Start-2021-Pre-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4A0C22-1B68-4125-8FEF-5D9EE3F26AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613B53F8-82A7-48F2-9B73-97884D29DCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF50913-B49A-43EC-88BB-5B5BBD86398F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="133">
   <si>
     <t>päivä</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t>Notification testit, redux fake store, store Provider wrapper</t>
+  </si>
+  <si>
+    <t>NoteAddEditInput testit, NoteAddEditInputCntr luotu API/store logiikan erotteluun, komponentin mockauksen opettelua</t>
+  </si>
+  <si>
+    <t>FavoritesList, FavoriteListItem testit</t>
+  </si>
+  <si>
+    <t>Etusivun viimeisiä kommentteja ennen palautusta</t>
   </si>
 </sst>
 </file>
@@ -792,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E0410-90FF-44A4-A927-CBAC5BD28BF8}">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,7 +2212,38 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="5">
+        <v>44596</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2</v>
+      </c>
+      <c r="C120" t="s">
+        <v>130</v>
+      </c>
       <c r="D120" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="1">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>131</v>
+      </c>
+      <c r="D121" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>132</v>
+      </c>
+      <c r="D122" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2212,8 +2252,8 @@
         <v>2</v>
       </c>
       <c r="B123" s="1">
-        <f>SUM(B2:B119)</f>
-        <v>171</v>
+        <f>SUM(B2:B122)</f>
+        <v>177</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2230,7 +2270,7 @@
       </c>
       <c r="B125" s="1">
         <f>B123/B124*100</f>
-        <v>97.714285714285708</v>
+        <v>101.14285714285714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>